<commit_message>
remove EF 2008 flex motorcycles
</commit_message>
<xml_diff>
--- a/projects/brazil_bu/config/inventory.xlsx
+++ b/projects/brazil_bu/config/inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
     <sheet name="tfs" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="mileage" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="fuel" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="met" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">fleet_age!$A$1:$AA$41</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="57">
   <si>
     <t xml:space="preserve">family</t>
   </si>
@@ -194,6 +194,12 @@
   <si>
     <t xml:space="preserve">consumption_lt</t>
   </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
 </sst>
 </file>
 
@@ -300,10 +306,10 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="I2:I17 A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.48"/>
@@ -765,10 +771,10 @@
   <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="1" sqref="I2:I17 E25"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4194,10 +4200,10 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="I2:I17 N2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="17.67"/>
@@ -6335,11 +6341,11 @@
   </sheetPr>
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2:I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="8.67"/>
@@ -9786,10 +9792,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="I2:I17 D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
@@ -9856,35 +9862,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I2:I17 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>18219.59</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>21109.92</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>21914.33</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>21277.16</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>19842.75</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>18255.44</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>17159.57</v>
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>16.9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>